<commit_message>
updated the last scores
</commit_message>
<xml_diff>
--- a/benchmark/summary.xlsx
+++ b/benchmark/summary.xlsx
@@ -174,7 +174,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -192,18 +192,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -227,14 +215,14 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topLeft" activeCell="L10" activeCellId="0" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.95"/>
@@ -329,12 +317,10 @@
         <v>0.689</v>
       </c>
       <c r="L2" s="1" t="n">
-        <f aca="false">ROUND(2*L3*L4/(L3+L4),3)</f>
-        <v>0.57</v>
+        <v>0.608</v>
       </c>
       <c r="M2" s="1" t="n">
-        <f aca="false">ROUND(2*M3*M4/(M3+M4),3)</f>
-        <v>0.63</v>
+        <v>0.632</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -372,10 +358,10 @@
         <v>0.691</v>
       </c>
       <c r="L3" s="1" t="n">
-        <v>0.578</v>
+        <v>0.604</v>
       </c>
       <c r="M3" s="1" t="n">
-        <v>0.625</v>
+        <v>0.631</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -413,10 +399,10 @@
         <v>0.688</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>0.563</v>
+        <v>0.613</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>0.636</v>
+        <v>0.633</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -432,7 +418,7 @@
       <c r="D5" s="1" t="n">
         <v>0.748</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="3" t="n">
         <v>0.83</v>
       </c>
       <c r="F5" s="1" t="n">
@@ -454,10 +440,10 @@
         <v>0.842</v>
       </c>
       <c r="L5" s="1" t="n">
-        <v>0.734</v>
+        <v>0.736</v>
       </c>
       <c r="M5" s="1" t="n">
-        <v>0.674</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -495,10 +481,10 @@
         <v>0.596</v>
       </c>
       <c r="L6" s="1" t="n">
-        <v>0.497</v>
+        <v>0.538</v>
       </c>
       <c r="M6" s="1" t="n">
-        <v>0.614</v>
+        <v>0.554</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -556,7 +542,6 @@
         <f aca="false">ROUND(2*D13*D14/(D13+D14),3)</f>
         <v>0.751</v>
       </c>
-      <c r="E12" s="6"/>
       <c r="F12" s="4" t="n">
         <f aca="false">ROUND(2*F13*F14/(F13+F14),3)</f>
         <v>0.789</v>
@@ -595,7 +580,6 @@
       <c r="D13" s="1" t="n">
         <v>0.746</v>
       </c>
-      <c r="E13" s="6"/>
       <c r="F13" s="4" t="n">
         <v>0.762</v>
       </c>
@@ -628,7 +612,6 @@
       <c r="D14" s="1" t="n">
         <v>0.757</v>
       </c>
-      <c r="E14" s="6"/>
       <c r="F14" s="4" t="n">
         <v>0.819</v>
       </c>
@@ -661,8 +644,7 @@
       <c r="D15" s="1" t="n">
         <v>0.804</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="5" t="n">
+      <c r="F15" s="3" t="n">
         <v>0.818</v>
       </c>
       <c r="G15" s="1" t="n">
@@ -694,7 +676,7 @@
       <c r="D16" s="1" t="n">
         <v>0.757</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="2"/>
       <c r="F16" s="4" t="n">
         <v>0.839</v>
       </c>
@@ -754,12 +736,10 @@
         <v>0.819</v>
       </c>
       <c r="L17" s="1" t="n">
-        <f aca="false">ROUND(2*L18*L19/(L18+L19),3)</f>
-        <v>0.669</v>
+        <v>0.729</v>
       </c>
       <c r="M17" s="1" t="n">
-        <f aca="false">ROUND(2*M18*M19/(M18+M19),3)</f>
-        <v>0.749</v>
+        <v>0.763</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -794,10 +774,10 @@
         <v>0.829</v>
       </c>
       <c r="L18" s="1" t="n">
-        <v>0.681</v>
+        <v>0.726</v>
       </c>
       <c r="M18" s="1" t="n">
-        <v>0.74</v>
+        <v>0.762</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -832,10 +812,10 @@
         <v>0.809</v>
       </c>
       <c r="L19" s="1" t="n">
-        <v>0.657</v>
+        <v>0.732</v>
       </c>
       <c r="M19" s="1" t="n">
-        <v>0.759</v>
+        <v>0.764</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -870,10 +850,10 @@
         <v>0.848</v>
       </c>
       <c r="L20" s="1" t="n">
-        <v>0.693</v>
+        <v>0.767</v>
       </c>
       <c r="M20" s="1" t="n">
-        <v>0.75</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -908,10 +888,10 @@
         <v>0.808</v>
       </c>
       <c r="L21" s="1" t="n">
-        <v>0.659</v>
+        <v>0.723</v>
       </c>
       <c r="M21" s="1" t="n">
-        <v>0.795</v>
+        <v>0.751</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
allow several parm sets + the new best
</commit_message>
<xml_diff>
--- a/benchmark/summary.xlsx
+++ b/benchmark/summary.xlsx
@@ -215,7 +215,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M18" activeCellId="0" sqref="M18"/>
+      <selection pane="topLeft" activeCell="N21" activeCellId="0" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -317,10 +317,10 @@
         <v>0.689</v>
       </c>
       <c r="L2" s="1" t="n">
-        <v>0.609</v>
+        <v>0.63</v>
       </c>
       <c r="M2" s="1" t="n">
-        <v>0.676</v>
+        <v>0.672</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -358,10 +358,10 @@
         <v>0.691</v>
       </c>
       <c r="L3" s="1" t="n">
-        <v>0.605</v>
+        <v>0.626</v>
       </c>
       <c r="M3" s="1" t="n">
-        <v>0.671</v>
+        <v>0.669</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -399,10 +399,10 @@
         <v>0.688</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>0.613</v>
+        <v>0.635</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>0.681</v>
+        <v>0.675</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -440,10 +440,10 @@
         <v>0.842</v>
       </c>
       <c r="L5" s="1" t="n">
-        <v>0.694</v>
+        <v>0.722</v>
       </c>
       <c r="M5" s="1" t="n">
-        <v>0.78</v>
+        <v>0.778</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -481,10 +481,10 @@
         <v>0.596</v>
       </c>
       <c r="L6" s="1" t="n">
-        <v>0.561</v>
+        <v>0.579</v>
       </c>
       <c r="M6" s="1" t="n">
-        <v>0.615</v>
+        <v>0.607</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -736,10 +736,10 @@
         <v>0.819</v>
       </c>
       <c r="L17" s="1" t="n">
-        <v>0.729</v>
+        <v>0.728</v>
       </c>
       <c r="M17" s="1" t="n">
-        <v>0.79</v>
+        <v>0.791</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -774,10 +774,10 @@
         <v>0.829</v>
       </c>
       <c r="L18" s="1" t="n">
-        <v>0.716</v>
+        <v>0.709</v>
       </c>
       <c r="M18" s="1" t="n">
-        <v>0.783</v>
+        <v>0.782</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,10 +812,10 @@
         <v>0.809</v>
       </c>
       <c r="L19" s="1" t="n">
-        <v>0.742</v>
+        <v>0.747</v>
       </c>
       <c r="M19" s="1" t="n">
-        <v>0.797</v>
+        <v>0.801</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,10 +850,10 @@
         <v>0.848</v>
       </c>
       <c r="L20" s="1" t="n">
-        <v>0.748</v>
+        <v>0.754</v>
       </c>
       <c r="M20" s="1" t="n">
-        <v>0.808</v>
+        <v>0.827</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -888,10 +888,10 @@
         <v>0.808</v>
       </c>
       <c r="L21" s="1" t="n">
-        <v>0.756</v>
+        <v>0.76</v>
       </c>
       <c r="M21" s="1" t="n">
-        <v>0.808</v>
+        <v>0.799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved to canonical-only SPOTRNA for CoRToise and CoRToise150
</commit_message>
<xml_diff>
--- a/benchmark/summary.xlsx
+++ b/benchmark/summary.xlsx
@@ -174,7 +174,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -192,6 +192,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -215,7 +223,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N21" activeCellId="0" sqref="N21"/>
+      <selection pane="topLeft" activeCell="K30" activeCellId="0" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -542,6 +550,10 @@
         <f aca="false">ROUND(2*D13*D14/(D13+D14),3)</f>
         <v>0.751</v>
       </c>
+      <c r="E12" s="1" t="n">
+        <f aca="false">ROUND(2*E13*E14/(E13+E14),3)</f>
+        <v>0.774</v>
+      </c>
       <c r="F12" s="4" t="n">
         <f aca="false">ROUND(2*F13*F14/(F13+F14),3)</f>
         <v>0.789</v>
@@ -580,6 +592,9 @@
       <c r="D13" s="1" t="n">
         <v>0.746</v>
       </c>
+      <c r="E13" s="1" t="n">
+        <v>0.734</v>
+      </c>
       <c r="F13" s="4" t="n">
         <v>0.762</v>
       </c>
@@ -612,6 +627,9 @@
       <c r="D14" s="1" t="n">
         <v>0.757</v>
       </c>
+      <c r="E14" s="5" t="n">
+        <v>0.818</v>
+      </c>
       <c r="F14" s="4" t="n">
         <v>0.819</v>
       </c>
@@ -627,7 +645,7 @@
       <c r="J14" s="1" t="n">
         <v>0.784</v>
       </c>
-      <c r="K14" s="4" t="n">
+      <c r="K14" s="6" t="n">
         <v>0.806</v>
       </c>
     </row>
@@ -644,6 +662,9 @@
       <c r="D15" s="1" t="n">
         <v>0.804</v>
       </c>
+      <c r="E15" s="1" t="n">
+        <v>0.843</v>
+      </c>
       <c r="F15" s="3" t="n">
         <v>0.818</v>
       </c>
@@ -676,7 +697,9 @@
       <c r="D16" s="1" t="n">
         <v>0.757</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="5" t="n">
+        <v>0.831</v>
+      </c>
       <c r="F16" s="4" t="n">
         <v>0.839</v>
       </c>
@@ -692,7 +715,7 @@
       <c r="J16" s="1" t="n">
         <v>0.768</v>
       </c>
-      <c r="K16" s="4" t="n">
+      <c r="K16" s="6" t="n">
         <v>0.803</v>
       </c>
     </row>
@@ -711,6 +734,10 @@
         <f aca="false">ROUND(2*D18*D19/(D18+D19),3)</f>
         <v>0.769</v>
       </c>
+      <c r="E17" s="5" t="n">
+        <f aca="false">ROUND(2*E18*E19/(E18+E19),3)</f>
+        <v>0.833</v>
+      </c>
       <c r="F17" s="4" t="n">
         <f aca="false">ROUND(2*F18*F19/(F18+F19),3)</f>
         <v>0.822</v>
@@ -731,7 +758,7 @@
         <f aca="false">ROUND(2*J18*J19/(J18+J19),3)</f>
         <v>0.808</v>
       </c>
-      <c r="K17" s="4" t="n">
+      <c r="K17" s="6" t="n">
         <f aca="false">ROUND(2*K18*K19/(K18+K19),3)</f>
         <v>0.819</v>
       </c>
@@ -755,6 +782,9 @@
       <c r="D18" s="1" t="n">
         <v>0.779</v>
       </c>
+      <c r="E18" s="5" t="n">
+        <v>0.843</v>
+      </c>
       <c r="F18" s="1" t="n">
         <v>0.822</v>
       </c>
@@ -770,7 +800,7 @@
       <c r="J18" s="4" t="n">
         <v>0.832</v>
       </c>
-      <c r="K18" s="4" t="n">
+      <c r="K18" s="6" t="n">
         <v>0.829</v>
       </c>
       <c r="L18" s="1" t="n">
@@ -793,6 +823,9 @@
       <c r="D19" s="1" t="n">
         <v>0.759</v>
       </c>
+      <c r="E19" s="5" t="n">
+        <v>0.824</v>
+      </c>
       <c r="F19" s="4" t="n">
         <v>0.822</v>
       </c>
@@ -808,7 +841,7 @@
       <c r="J19" s="1" t="n">
         <v>0.786</v>
       </c>
-      <c r="K19" s="4" t="n">
+      <c r="K19" s="6" t="n">
         <v>0.809</v>
       </c>
       <c r="L19" s="1" t="n">
@@ -831,6 +864,9 @@
       <c r="D20" s="1" t="n">
         <v>0.806</v>
       </c>
+      <c r="E20" s="1" t="n">
+        <v>0.847</v>
+      </c>
       <c r="F20" s="1" t="n">
         <v>0.821</v>
       </c>
@@ -869,6 +905,9 @@
       <c r="D21" s="1" t="n">
         <v>0.759</v>
       </c>
+      <c r="E21" s="5" t="n">
+        <v>0.84</v>
+      </c>
       <c r="F21" s="4" t="n">
         <v>0.842</v>
       </c>
@@ -884,7 +923,7 @@
       <c r="J21" s="1" t="n">
         <v>0.772</v>
       </c>
-      <c r="K21" s="4" t="n">
+      <c r="K21" s="6" t="n">
         <v>0.808</v>
       </c>
       <c r="L21" s="1" t="n">

</xml_diff>

<commit_message>
added ScoreStruct for rankings -> new best scores
</commit_message>
<xml_diff>
--- a/benchmark/summary.xlsx
+++ b/benchmark/summary.xlsx
@@ -174,7 +174,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -199,7 +199,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -223,7 +227,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N17" activeCellId="0" sqref="N17"/>
+      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -324,12 +328,6 @@
         <f aca="false">ROUND(2*K3*K4/(K3+K4),3)</f>
         <v>0.689</v>
       </c>
-      <c r="L2" s="1" t="n">
-        <v>0.623</v>
-      </c>
-      <c r="M2" s="1" t="n">
-        <v>0.677</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -365,12 +363,6 @@
       <c r="K3" s="4" t="n">
         <v>0.691</v>
       </c>
-      <c r="L3" s="1" t="n">
-        <v>0.621</v>
-      </c>
-      <c r="M3" s="1" t="n">
-        <v>0.673</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -406,12 +398,6 @@
       <c r="K4" s="4" t="n">
         <v>0.688</v>
       </c>
-      <c r="L4" s="1" t="n">
-        <v>0.626</v>
-      </c>
-      <c r="M4" s="1" t="n">
-        <v>0.681</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -447,12 +433,6 @@
       <c r="K5" s="4" t="n">
         <v>0.842</v>
       </c>
-      <c r="L5" s="1" t="n">
-        <v>0.685</v>
-      </c>
-      <c r="M5" s="1" t="n">
-        <v>0.771</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -470,7 +450,7 @@
       <c r="E6" s="4" t="n">
         <v>0.66</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="5" t="n">
         <v>0.609</v>
       </c>
       <c r="G6" s="1" t="n">
@@ -488,12 +468,7 @@
       <c r="K6" s="2" t="n">
         <v>0.596</v>
       </c>
-      <c r="L6" s="1" t="n">
-        <v>0.587</v>
-      </c>
-      <c r="M6" s="5" t="n">
-        <v>0.618</v>
-      </c>
+      <c r="M6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
@@ -510,19 +485,19 @@
         <f aca="false">ROUND(2*D8*D9/(D8+D9),3)</f>
         <v>0.712</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="4" t="n">
         <f aca="false">ROUND(2*E8*E9/(E8+E9),3)</f>
         <v>0.792</v>
       </c>
-      <c r="F7" s="6" t="n">
+      <c r="F7" s="7" t="n">
         <f aca="false">ROUND(2*F8*F9/(F8+F9),3)</f>
         <v>0.753</v>
       </c>
       <c r="L7" s="1" t="n">
-        <v>0.688</v>
-      </c>
-      <c r="M7" s="1" t="n">
-        <v>0.75</v>
+        <v>0.714</v>
+      </c>
+      <c r="M7" s="5" t="n">
+        <v>0.761</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -538,17 +513,17 @@
       <c r="D8" s="1" t="n">
         <v>0.714</v>
       </c>
-      <c r="E8" s="6" t="n">
+      <c r="E8" s="4" t="n">
         <v>0.796</v>
       </c>
-      <c r="F8" s="6" t="n">
+      <c r="F8" s="7" t="n">
         <v>0.756</v>
       </c>
       <c r="L8" s="1" t="n">
-        <v>0.69</v>
-      </c>
-      <c r="M8" s="1" t="n">
-        <v>0.749</v>
+        <v>0.717</v>
+      </c>
+      <c r="M8" s="5" t="n">
+        <v>0.759</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -564,17 +539,17 @@
       <c r="D9" s="1" t="n">
         <v>0.711</v>
       </c>
-      <c r="E9" s="6" t="n">
+      <c r="E9" s="4" t="n">
         <v>0.789</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>0.75</v>
       </c>
       <c r="L9" s="1" t="n">
-        <v>0.687</v>
-      </c>
-      <c r="M9" s="6" t="n">
-        <v>0.751</v>
+        <v>0.711</v>
+      </c>
+      <c r="M9" s="4" t="n">
+        <v>0.763</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -590,17 +565,17 @@
       <c r="D10" s="1" t="n">
         <v>0.748</v>
       </c>
-      <c r="E10" s="6" t="n">
+      <c r="E10" s="4" t="n">
         <v>0.847</v>
       </c>
-      <c r="F10" s="6" t="n">
+      <c r="F10" s="7" t="n">
         <v>0.777</v>
       </c>
       <c r="L10" s="1" t="n">
-        <v>0.685</v>
-      </c>
-      <c r="M10" s="1" t="n">
-        <v>0.773</v>
+        <v>0.717</v>
+      </c>
+      <c r="M10" s="5" t="n">
+        <v>0.783</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -616,17 +591,17 @@
       <c r="D11" s="1" t="n">
         <v>0.688</v>
       </c>
-      <c r="E11" s="6" t="n">
+      <c r="E11" s="4" t="n">
         <v>0.753</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>0.736</v>
       </c>
       <c r="L11" s="1" t="n">
-        <v>0.703</v>
-      </c>
-      <c r="M11" s="6" t="n">
-        <v>0.74</v>
+        <v>0.721</v>
+      </c>
+      <c r="M11" s="4" t="n">
+        <v>0.754</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -832,7 +807,7 @@
         <f aca="false">ROUND(2*E18*E19/(E18+E19),3)</f>
         <v>0.833</v>
       </c>
-      <c r="F17" s="4" t="n">
+      <c r="F17" s="7" t="n">
         <f aca="false">ROUND(2*F18*F19/(F18+F19),3)</f>
         <v>0.822</v>
       </c>
@@ -857,10 +832,10 @@
         <v>0.819</v>
       </c>
       <c r="L17" s="1" t="n">
-        <v>0.738</v>
-      </c>
-      <c r="M17" s="1" t="n">
-        <v>0.817</v>
+        <v>0.757</v>
+      </c>
+      <c r="M17" s="5" t="n">
+        <v>0.827</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -898,10 +873,10 @@
         <v>0.829</v>
       </c>
       <c r="L18" s="1" t="n">
-        <v>0.721</v>
+        <v>0.743</v>
       </c>
       <c r="M18" s="1" t="n">
-        <v>0.804</v>
+        <v>0.816</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -939,10 +914,10 @@
         <v>0.809</v>
       </c>
       <c r="L19" s="1" t="n">
-        <v>0.756</v>
+        <v>0.771</v>
       </c>
       <c r="M19" s="5" t="n">
-        <v>0.831</v>
+        <v>0.838</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -980,10 +955,10 @@
         <v>0.848</v>
       </c>
       <c r="L20" s="1" t="n">
-        <v>0.73</v>
+        <v>0.754</v>
       </c>
       <c r="M20" s="1" t="n">
-        <v>0.838</v>
+        <v>0.843</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,10 +996,10 @@
         <v>0.808</v>
       </c>
       <c r="L21" s="1" t="n">
-        <v>0.805</v>
+        <v>0.808</v>
       </c>
       <c r="M21" s="5" t="n">
-        <v>0.844</v>
+        <v>0.853</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove ExtendStems and roll back
</commit_message>
<xml_diff>
--- a/benchmark/summary.xlsx
+++ b/benchmark/summary.xlsx
@@ -223,7 +223,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12"/>
+      <selection pane="topLeft" activeCell="I26" activeCellId="0" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -490,10 +490,10 @@
         <v>0.753</v>
       </c>
       <c r="L7" s="1" t="n">
-        <v>0.708</v>
+        <v>0.714</v>
       </c>
       <c r="M7" s="5" t="n">
-        <v>0.758</v>
+        <v>0.761</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -516,10 +516,10 @@
         <v>0.756</v>
       </c>
       <c r="L8" s="1" t="n">
-        <v>0.713</v>
+        <v>0.717</v>
       </c>
       <c r="M8" s="5" t="n">
-        <v>0.757</v>
+        <v>0.759</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -542,10 +542,10 @@
         <v>0.75</v>
       </c>
       <c r="L9" s="1" t="n">
-        <v>0.704</v>
+        <v>0.711</v>
       </c>
       <c r="M9" s="4" t="n">
-        <v>0.76</v>
+        <v>0.763</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,10 +568,10 @@
         <v>0.777</v>
       </c>
       <c r="L10" s="1" t="n">
-        <v>0.709</v>
+        <v>0.717</v>
       </c>
       <c r="M10" s="5" t="n">
-        <v>0.777</v>
+        <v>0.783</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -594,10 +594,10 @@
         <v>0.736</v>
       </c>
       <c r="L11" s="1" t="n">
-        <v>0.715</v>
+        <v>0.721</v>
       </c>
       <c r="M11" s="4" t="n">
-        <v>0.753</v>
+        <v>0.754</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -828,10 +828,10 @@
         <v>0.819</v>
       </c>
       <c r="L17" s="1" t="n">
-        <v>0.759</v>
+        <v>0.757</v>
       </c>
       <c r="M17" s="5" t="n">
-        <v>0.828</v>
+        <v>0.827</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,10 +869,10 @@
         <v>0.829</v>
       </c>
       <c r="L18" s="1" t="n">
-        <v>0.746</v>
+        <v>0.743</v>
       </c>
       <c r="M18" s="1" t="n">
-        <v>0.818</v>
+        <v>0.816</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -910,10 +910,10 @@
         <v>0.809</v>
       </c>
       <c r="L19" s="1" t="n">
-        <v>0.772</v>
+        <v>0.771</v>
       </c>
       <c r="M19" s="5" t="n">
-        <v>0.839</v>
+        <v>0.838</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -951,10 +951,10 @@
         <v>0.848</v>
       </c>
       <c r="L20" s="1" t="n">
-        <v>0.755</v>
+        <v>0.754</v>
       </c>
       <c r="M20" s="1" t="n">
-        <v>0.844</v>
+        <v>0.843</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -992,10 +992,10 @@
         <v>0.808</v>
       </c>
       <c r="L21" s="1" t="n">
-        <v>0.81</v>
+        <v>0.808</v>
       </c>
       <c r="M21" s="5" t="n">
-        <v>0.854</v>
+        <v>0.853</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove gupen + roll back
</commit_message>
<xml_diff>
--- a/benchmark/summary.xlsx
+++ b/benchmark/summary.xlsx
@@ -223,7 +223,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I26" activeCellId="0" sqref="I26"/>
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -490,10 +490,10 @@
         <v>0.753</v>
       </c>
       <c r="L7" s="1" t="n">
-        <v>0.714</v>
+        <v>0.712</v>
       </c>
       <c r="M7" s="5" t="n">
-        <v>0.761</v>
+        <v>0.766</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -516,10 +516,10 @@
         <v>0.756</v>
       </c>
       <c r="L8" s="1" t="n">
-        <v>0.717</v>
+        <v>0.715</v>
       </c>
       <c r="M8" s="5" t="n">
-        <v>0.759</v>
+        <v>0.766</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -542,10 +542,10 @@
         <v>0.75</v>
       </c>
       <c r="L9" s="1" t="n">
-        <v>0.711</v>
+        <v>0.71</v>
       </c>
       <c r="M9" s="4" t="n">
-        <v>0.763</v>
+        <v>0.767</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,10 +568,10 @@
         <v>0.777</v>
       </c>
       <c r="L10" s="1" t="n">
-        <v>0.717</v>
+        <v>0.718</v>
       </c>
       <c r="M10" s="5" t="n">
-        <v>0.783</v>
+        <v>0.789</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -594,10 +594,10 @@
         <v>0.736</v>
       </c>
       <c r="L11" s="1" t="n">
-        <v>0.721</v>
+        <v>0.718</v>
       </c>
       <c r="M11" s="4" t="n">
-        <v>0.754</v>
+        <v>0.757</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -828,10 +828,10 @@
         <v>0.819</v>
       </c>
       <c r="L17" s="1" t="n">
-        <v>0.757</v>
+        <v>0.755</v>
       </c>
       <c r="M17" s="5" t="n">
-        <v>0.827</v>
+        <v>0.826</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,10 +869,10 @@
         <v>0.829</v>
       </c>
       <c r="L18" s="1" t="n">
-        <v>0.743</v>
+        <v>0.741</v>
       </c>
       <c r="M18" s="1" t="n">
-        <v>0.816</v>
+        <v>0.815</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -910,7 +910,7 @@
         <v>0.809</v>
       </c>
       <c r="L19" s="1" t="n">
-        <v>0.771</v>
+        <v>0.77</v>
       </c>
       <c r="M19" s="5" t="n">
         <v>0.838</v>
@@ -954,7 +954,7 @@
         <v>0.754</v>
       </c>
       <c r="M20" s="1" t="n">
-        <v>0.843</v>
+        <v>0.842</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,7 +995,7 @@
         <v>0.808</v>
       </c>
       <c r="M21" s="5" t="n">
-        <v>0.853</v>
+        <v>0.852</v>
       </c>
     </row>
   </sheetData>

</xml_diff>